<commit_message>
2D Gaussian with Different Fixed-Point Formats
</commit_message>
<xml_diff>
--- a/Results/Results_python.xlsx
+++ b/Results/Results_python.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5927951\Documents\Univali\TTC\TTCIII\Project\Architecture-of-FPGA-based-Systems-for-Digital-Image-Processing\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05786A00-FE5A-458F-BBE6-220E241FC5E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A99D37-0E07-4FFD-9D71-85389EF08048}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-4470" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Virtual Board" sheetId="1" r:id="rId1"/>
     <sheet name="Fixed-Float SW" sheetId="2" r:id="rId2"/>
+    <sheet name="HW Sim-Gaussian 2D-FX" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">('HW Sim-Gaussian 2D-FX'!$B$5,'HW Sim-Gaussian 2D-FX'!$O$5,'HW Sim-Gaussian 2D-FX'!$AB$5)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">('HW Sim-Gaussian 2D-FX'!$B$5,'HW Sim-Gaussian 2D-FX'!$O$5,'HW Sim-Gaussian 2D-FX'!$AB$5)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">('HW Sim-Gaussian 2D-FX'!$B$5,'HW Sim-Gaussian 2D-FX'!$O$5,'HW Sim-Gaussian 2D-FX'!$AB$5)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="30">
   <si>
     <t>Black</t>
   </si>
@@ -78,16 +84,62 @@
   <si>
     <t>Comparison Between Fixed-Point Gaussian and Floating-Point Gaussian with Virtual Board 0 Approach</t>
   </si>
+  <si>
+    <t>Silicon Costs</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>ALM</t>
+  </si>
+  <si>
+    <t>Registers</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
+    <t>Memory Bits</t>
+  </si>
+  <si>
+    <t>DSP blocks</t>
+  </si>
+  <si>
+    <t>Relative (%)</t>
+  </si>
+  <si>
+    <t>Freq (MHz)</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - Fixed Point - 16 bits (8.8)</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - Fixed Point - 14 bits (8.6)</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - Fixed Point - 12 bits (8.4)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +192,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +228,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,10 +357,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +410,30 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,36 +467,73 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,6 +546,2516 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Custo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de Silício - Filtro Gaussiano - Ponto Fixo 16 bits</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ALM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>('HW Sim-Gaussian 2D-FX'!$A$5,'HW Sim-Gaussian 2D-FX'!$A$6,'HW Sim-Gaussian 2D-FX'!$A$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.7664483941378235E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.234798877455566E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1078889928281882E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-78C3-4B3C-B4AA-AC803CF5DBFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Registers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>('HW Sim-Gaussian 2D-FX'!$A$5,'HW Sim-Gaussian 2D-FX'!$A$6,'HW Sim-Gaussian 2D-FX'!$A$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$G$5:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.647700701480904E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4045206547155105E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3265783320342946E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-78C3-4B3C-B4AA-AC803CF5DBFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory Bits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>('HW Sim-Gaussian 2D-FX'!$A$5,'HW Sim-Gaussian 2D-FX'!$A$6,'HW Sim-Gaussian 2D-FX'!$A$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$H$5:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.02235516372796E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0447103274559201E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2067065491183878E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-78C3-4B3C-B4AA-AC803CF5DBFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DSP blocks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>('HW Sim-Gaussian 2D-FX'!$A$5,'HW Sim-Gaussian 2D-FX'!$A$6,'HW Sim-Gaussian 2D-FX'!$A$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HW Sim-Gaussian 2D-FX'!$I$5:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.1954022988505746E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26436781609195403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52873563218390807</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-78C3-4B3C-B4AA-AC803CF5DBFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="501402024"/>
+        <c:axId val="501399728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="501402024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Altura da Janela</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501399728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="501399728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Porcentagem de Utilização</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501402024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Utilização de ALMs por Dimensão</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de Janela e Número de Bits</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>7x7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>676</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>604</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>532</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B27F-4B81-A952-DA0227FBA0FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>5x5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>396</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>362</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>325</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B27F-4B81-A952-DA0227FBA0FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3x3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>12</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('HW Sim-Gaussian 2D-FX'!$B$5,'HW Sim-Gaussian 2D-FX'!$O$5,'HW Sim-Gaussian 2D-FX'!$AB$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B27F-4B81-A952-DA0227FBA0FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="501872096"/>
+        <c:axId val="501871768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="501872096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Número de Bits</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501871768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="501871768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501872096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88E54C79-1458-4979-A040-1AC1F1775F39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10FDBD89-8D8A-4A1D-BFCA-F250647529E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -715,7 +3358,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:S7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,93 +3385,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="18" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="19"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="27"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="34"/>
+      <c r="J3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="20" t="s">
+      <c r="M3" s="34"/>
+      <c r="N3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="20" t="s">
+      <c r="O3" s="29"/>
+      <c r="P3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="20" t="s">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="21"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1091,8 +3734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BA4AD1-F16F-4A97-9130-DD46CA139F38}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,93 +3762,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="18" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="19"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="27"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="34"/>
+      <c r="J3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="20" t="s">
+      <c r="M3" s="34"/>
+      <c r="N3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="20" t="s">
+      <c r="O3" s="29"/>
+      <c r="P3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="20" t="s">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="21"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1270,58 +3913,58 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="18">
         <v>6.24328488249907E-2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="19">
         <v>29.806451532821399</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="18">
         <v>6.22047424238601E-2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="19">
         <v>29.850070612916699</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="18">
         <v>6.2236136628961901E-2</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="19">
         <v>29.847346999427302</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="18">
         <v>6.2419029653738203E-2</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="19">
         <v>30.0987311261195</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="18">
         <v>6.3197749317954605E-2</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="19">
         <v>30.006350744827198</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="18">
         <v>6.3273997830548503E-2</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="19">
         <v>29.9977335029198</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="20">
         <v>6.2418019268688001E-2</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="21">
         <v>29.670245886255401</v>
       </c>
-      <c r="P5" s="31">
+      <c r="P5" s="20">
         <v>6.4169193778878406E-2</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="21">
         <v>29.450233917087498</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="20">
         <v>6.4472119797697194E-2</v>
       </c>
-      <c r="S5" s="32">
+      <c r="S5" s="21">
         <v>29.411539629982599</v>
       </c>
     </row>
@@ -1329,58 +3972,58 @@
       <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="18">
         <v>1.5597642543923601E-2</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="19">
         <v>41.853535314472097</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="18">
         <v>3.1231509815837898E-2</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="19">
         <v>35.8346809408268</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="18">
         <v>3.10873932346203E-2</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="19">
         <v>35.876513375305898</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="18">
         <v>1.55950641438989E-2</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="19">
         <v>42.145328077913803</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="18">
         <v>3.1248781776468101E-2</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="19">
         <v>36.123721158927196</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="18">
         <v>3.1098582342080901E-2</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="19">
         <v>36.1674271734</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="20">
         <v>1.5592061875617701E-2</v>
       </c>
-      <c r="O6" s="32">
+      <c r="O6" s="21">
         <v>41.718374553665001</v>
       </c>
-      <c r="P6" s="31">
+      <c r="P6" s="20">
         <v>3.1298597757026099E-2</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="21">
         <v>35.686267960633401</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="20">
         <v>3.11493936082929E-2</v>
       </c>
-      <c r="S6" s="32">
+      <c r="S6" s="21">
         <v>37.729986693273197</v>
       </c>
     </row>
@@ -1388,58 +4031,58 @@
       <c r="A7" s="5">
         <v>8</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="22">
         <v>9.1099583176323695E-5</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="23">
         <v>86.524386782097693</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="22">
         <v>1.17150775344403E-2</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="23">
         <v>44.351637189953301</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="22">
         <v>1.16011291747098E-2</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="23">
         <v>44.438194259541199</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="22">
         <v>1.6731987363879E-4</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="23">
         <v>81.534120827168394</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="22">
         <v>1.17186253759935E-2</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="23">
         <v>44.642849565703699</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="22">
         <v>1.16018737436418E-2</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="23">
         <v>44.731676308845302</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="24">
         <v>2.8127739436782401E-4</v>
       </c>
-      <c r="O7" s="36">
+      <c r="O7" s="25">
         <v>76.593748939133505</v>
       </c>
-      <c r="P7" s="35">
+      <c r="P7" s="24">
         <v>1.17272098952665E-2</v>
       </c>
-      <c r="Q7" s="36">
+      <c r="Q7" s="25">
         <v>44.212871608450101</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="24">
         <v>1.16612230471264E-2</v>
       </c>
-      <c r="S7" s="36">
+      <c r="S7" s="25">
         <v>44.264096579018997</v>
       </c>
     </row>
@@ -1461,4 +4104,710 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2859E3E8-E749-4A59-9466-92E0E94C8F86}">
+  <dimension ref="A1:AL7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.85546875" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="40"/>
+      <c r="N1" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="40"/>
+      <c r="AA1" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="40"/>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="N2" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="43"/>
+      <c r="AA2" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK2" s="42"/>
+      <c r="AL2" s="43"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="47"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC3" s="45"/>
+      <c r="AD3" s="45"/>
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="45"/>
+      <c r="AI3" s="45"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="47"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF4" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ4" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK4" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL4" s="51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
+        <v>3</v>
+      </c>
+      <c r="B5" s="52">
+        <v>217</v>
+      </c>
+      <c r="C5" s="52">
+        <v>468</v>
+      </c>
+      <c r="D5" s="52">
+        <v>16352</v>
+      </c>
+      <c r="E5" s="52">
+        <v>8</v>
+      </c>
+      <c r="F5" s="53">
+        <f>B5/32070</f>
+        <v>6.7664483941378235E-3</v>
+      </c>
+      <c r="G5" s="53">
+        <f>C5/128300</f>
+        <v>3.647700701480904E-3</v>
+      </c>
+      <c r="H5" s="53">
+        <f>D5/4065280</f>
+        <v>4.02235516372796E-3</v>
+      </c>
+      <c r="I5" s="53">
+        <f>E5/87</f>
+        <v>9.1954022988505746E-2</v>
+      </c>
+      <c r="J5" s="54">
+        <v>242.01</v>
+      </c>
+      <c r="K5" s="52">
+        <f>(512+A5-1)*(512+A5-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="L5" s="55">
+        <f>((1/(J5*10000000))*K5)*10000</f>
+        <v>1.0916904260154539</v>
+      </c>
+      <c r="N5" s="48">
+        <v>3</v>
+      </c>
+      <c r="O5" s="52">
+        <v>192</v>
+      </c>
+      <c r="P5" s="52">
+        <v>435</v>
+      </c>
+      <c r="Q5" s="52">
+        <v>14308</v>
+      </c>
+      <c r="R5" s="52">
+        <v>8</v>
+      </c>
+      <c r="S5" s="53">
+        <f>O5/32070</f>
+        <v>5.9869036482694104E-3</v>
+      </c>
+      <c r="T5" s="53">
+        <f>P5/128300</f>
+        <v>3.3904910366328918E-3</v>
+      </c>
+      <c r="U5" s="53">
+        <f>Q5/4065280</f>
+        <v>3.5195607682619646E-3</v>
+      </c>
+      <c r="V5" s="53">
+        <f>R5/87</f>
+        <v>9.1954022988505746E-2</v>
+      </c>
+      <c r="W5" s="54">
+        <v>267.24</v>
+      </c>
+      <c r="X5" s="52">
+        <f>(512+N5-1)*(512+N5-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="Y5" s="55">
+        <f>((1/(W5*10000000))*X5)*10000</f>
+        <v>0.98862445741655436</v>
+      </c>
+      <c r="AA5" s="48">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="52">
+        <v>187</v>
+      </c>
+      <c r="AC5" s="52">
+        <v>397</v>
+      </c>
+      <c r="AD5" s="52">
+        <v>12264</v>
+      </c>
+      <c r="AE5" s="52">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="53">
+        <f>AB5/32070</f>
+        <v>5.8309946990957283E-3</v>
+      </c>
+      <c r="AG5" s="53">
+        <f>AC5/128300</f>
+        <v>3.0943102104442712E-3</v>
+      </c>
+      <c r="AH5" s="53">
+        <f>AD5/4065280</f>
+        <v>3.0167663727959696E-3</v>
+      </c>
+      <c r="AI5" s="53">
+        <f>AE5/87</f>
+        <v>9.1954022988505746E-2</v>
+      </c>
+      <c r="AJ5" s="54">
+        <v>248.32</v>
+      </c>
+      <c r="AK5" s="52">
+        <f>(512+AA5-1)*(512+AA5-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="AL5" s="55">
+        <f>((1/(AJ5*10000000))*AK5)*10000</f>
+        <v>1.0639497422680413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
+        <v>5</v>
+      </c>
+      <c r="B6" s="52">
+        <v>396</v>
+      </c>
+      <c r="C6" s="52">
+        <v>950</v>
+      </c>
+      <c r="D6" s="52">
+        <v>32704</v>
+      </c>
+      <c r="E6" s="52">
+        <v>23</v>
+      </c>
+      <c r="F6" s="53">
+        <f t="shared" ref="F6:F7" si="0">B6/32070</f>
+        <v>1.234798877455566E-2</v>
+      </c>
+      <c r="G6" s="53">
+        <f t="shared" ref="G6:G7" si="1">C6/128300</f>
+        <v>7.4045206547155105E-3</v>
+      </c>
+      <c r="H6" s="53">
+        <f t="shared" ref="H6:H7" si="2">D6/4065280</f>
+        <v>8.0447103274559201E-3</v>
+      </c>
+      <c r="I6" s="53">
+        <f t="shared" ref="I6:I7" si="3">E6/87</f>
+        <v>0.26436781609195403</v>
+      </c>
+      <c r="J6" s="54">
+        <v>242.42</v>
+      </c>
+      <c r="K6" s="52">
+        <f t="shared" ref="K6:K7" si="4">(512+A6-1)*(512+A6-1)+4</f>
+        <v>266260</v>
+      </c>
+      <c r="L6" s="55">
+        <f t="shared" ref="L6:L7" si="5">((1/(J6*10000000))*K6)*10000</f>
+        <v>1.0983417209801172</v>
+      </c>
+      <c r="N6" s="48">
+        <v>5</v>
+      </c>
+      <c r="O6" s="52">
+        <v>362</v>
+      </c>
+      <c r="P6" s="52">
+        <v>852</v>
+      </c>
+      <c r="Q6" s="52">
+        <v>28616</v>
+      </c>
+      <c r="R6" s="52">
+        <v>23</v>
+      </c>
+      <c r="S6" s="53">
+        <f t="shared" ref="S6:S7" si="6">O6/32070</f>
+        <v>1.1287807920174617E-2</v>
+      </c>
+      <c r="T6" s="53">
+        <f t="shared" ref="T6:T7" si="7">P6/128300</f>
+        <v>6.6406858924395948E-3</v>
+      </c>
+      <c r="U6" s="53">
+        <f t="shared" ref="U6:U7" si="8">Q6/4065280</f>
+        <v>7.0391215365239292E-3</v>
+      </c>
+      <c r="V6" s="53">
+        <f t="shared" ref="V6:V7" si="9">R6/87</f>
+        <v>0.26436781609195403</v>
+      </c>
+      <c r="W6" s="54">
+        <v>254.26</v>
+      </c>
+      <c r="X6" s="52">
+        <f>(512+N6-1)*(512+N6-1)+4</f>
+        <v>266260</v>
+      </c>
+      <c r="Y6" s="55">
+        <f t="shared" ref="Y6:Y7" si="10">((1/(W6*10000000))*X6)*10000</f>
+        <v>1.0471957838433099</v>
+      </c>
+      <c r="AA6" s="48">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="52">
+        <v>325</v>
+      </c>
+      <c r="AC6" s="52">
+        <v>758</v>
+      </c>
+      <c r="AD6" s="52">
+        <v>24528</v>
+      </c>
+      <c r="AE6" s="52">
+        <v>23</v>
+      </c>
+      <c r="AF6" s="53">
+        <f t="shared" ref="AF6:AF7" si="11">AB6/32070</f>
+        <v>1.0134081696289368E-2</v>
+      </c>
+      <c r="AG6" s="53">
+        <f t="shared" ref="AG6:AG7" si="12">AC6/128300</f>
+        <v>5.9080280592361655E-3</v>
+      </c>
+      <c r="AH6" s="53">
+        <f t="shared" ref="AH6:AH7" si="13">AD6/4065280</f>
+        <v>6.0335327455919392E-3</v>
+      </c>
+      <c r="AI6" s="53">
+        <f t="shared" ref="AI6:AI7" si="14">AE6/87</f>
+        <v>0.26436781609195403</v>
+      </c>
+      <c r="AJ6" s="54">
+        <v>241.14</v>
+      </c>
+      <c r="AK6" s="52">
+        <f>(512+AA6-1)*(512+AA6-1)+4</f>
+        <v>266260</v>
+      </c>
+      <c r="AL6" s="55">
+        <f t="shared" ref="AL6:AL7" si="15">((1/(AJ6*10000000))*AK6)*10000</f>
+        <v>1.1041718503773741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="49">
+        <v>7</v>
+      </c>
+      <c r="B7" s="56">
+        <v>676</v>
+      </c>
+      <c r="C7" s="56">
+        <v>1702</v>
+      </c>
+      <c r="D7" s="56">
+        <v>49056</v>
+      </c>
+      <c r="E7" s="56">
+        <v>46</v>
+      </c>
+      <c r="F7" s="57">
+        <f t="shared" si="0"/>
+        <v>2.1078889928281882E-2</v>
+      </c>
+      <c r="G7" s="57">
+        <f t="shared" si="1"/>
+        <v>1.3265783320342946E-2</v>
+      </c>
+      <c r="H7" s="57">
+        <f t="shared" si="2"/>
+        <v>1.2067065491183878E-2</v>
+      </c>
+      <c r="I7" s="57">
+        <f t="shared" si="3"/>
+        <v>0.52873563218390807</v>
+      </c>
+      <c r="J7" s="58">
+        <v>225.48</v>
+      </c>
+      <c r="K7" s="56">
+        <f t="shared" si="4"/>
+        <v>268328</v>
+      </c>
+      <c r="L7" s="59">
+        <f t="shared" si="5"/>
+        <v>1.1900301578854</v>
+      </c>
+      <c r="N7" s="49">
+        <v>7</v>
+      </c>
+      <c r="O7" s="56">
+        <v>604</v>
+      </c>
+      <c r="P7" s="56">
+        <v>1518</v>
+      </c>
+      <c r="Q7" s="56">
+        <v>42924</v>
+      </c>
+      <c r="R7" s="56">
+        <v>46</v>
+      </c>
+      <c r="S7" s="57">
+        <f t="shared" si="6"/>
+        <v>1.8833801060180854E-2</v>
+      </c>
+      <c r="T7" s="57">
+        <f t="shared" si="7"/>
+        <v>1.1831644583008574E-2</v>
+      </c>
+      <c r="U7" s="57">
+        <f t="shared" si="8"/>
+        <v>1.0558682304785894E-2</v>
+      </c>
+      <c r="V7" s="57">
+        <f t="shared" si="9"/>
+        <v>0.52873563218390807</v>
+      </c>
+      <c r="W7" s="58">
+        <v>238.04</v>
+      </c>
+      <c r="X7" s="56">
+        <f>(512+N7-1)*(512+N7-1)+4</f>
+        <v>268328</v>
+      </c>
+      <c r="Y7" s="59">
+        <f t="shared" si="10"/>
+        <v>1.1272391194757185</v>
+      </c>
+      <c r="AA7" s="49">
+        <v>7</v>
+      </c>
+      <c r="AB7" s="56">
+        <v>532</v>
+      </c>
+      <c r="AC7" s="56">
+        <v>1325</v>
+      </c>
+      <c r="AD7" s="56">
+        <v>36792</v>
+      </c>
+      <c r="AE7" s="56">
+        <v>46</v>
+      </c>
+      <c r="AF7" s="57">
+        <f t="shared" si="11"/>
+        <v>1.6588712192079826E-2</v>
+      </c>
+      <c r="AG7" s="57">
+        <f t="shared" si="12"/>
+        <v>1.0327357755261106E-2</v>
+      </c>
+      <c r="AH7" s="57">
+        <f t="shared" si="13"/>
+        <v>9.0502991183879101E-3</v>
+      </c>
+      <c r="AI7" s="57">
+        <f t="shared" si="14"/>
+        <v>0.52873563218390807</v>
+      </c>
+      <c r="AJ7" s="58">
+        <v>230.52</v>
+      </c>
+      <c r="AK7" s="56">
+        <f>(512+AA7-1)*(512+AA7-1)+4</f>
+        <v>268328</v>
+      </c>
+      <c r="AL7" s="59">
+        <f t="shared" si="15"/>
+        <v>1.1640117994100294</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AA2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AF3:AI3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="N1:Y1"/>
+    <mergeCell ref="N2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Problem with Modified Filter - 2D Gaussian 3
</commit_message>
<xml_diff>
--- a/Results/Results_python.xlsx
+++ b/Results/Results_python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5927951\Documents\Univali\TTC\TTCIII\Project\Architecture-of-FPGA-based-Systems-for-Digital-Image-Processing\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A99D37-0E07-4FFD-9D71-85389EF08048}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F8A1A-3B47-47C1-AF60-613113D5B01A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
   </bookViews>
@@ -4111,7 +4111,7 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,7 +4807,94 @@
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="A1:L1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F5:I7">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{14F69937-56DF-4729-81F7-4936422AA226}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5:V7">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{01C2C581-3201-4A6A-A658-22099120F5C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF5:AI7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FE0B3B72-1135-4092-AEF5-FB16743EE543}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{14F69937-56DF-4729-81F7-4936422AA226}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F5:I7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{01C2C581-3201-4A6A-A658-22099120F5C3}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S5:V7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FE0B3B72-1135-4092-AEF5-FB16743EE543}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AF5:AI7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tests with APX filters (3x3)
</commit_message>
<xml_diff>
--- a/Results/Results_python.xlsx
+++ b/Results/Results_python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5927951\Documents\Univali\TTC\TTCIII\Project\Architecture-of-FPGA-based-Systems-for-Digital-Image-Processing\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD96DE1-129F-41EC-9E53-D75423CBFB97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BB821C-DD8B-446A-A178-CF8AF69D0B33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-4470" windowWidth="25440" windowHeight="15540" activeTab="4" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
+    <workbookView xWindow="-25320" yWindow="-4470" windowWidth="25440" windowHeight="15540" activeTab="5" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Virtual Board" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Gaussian 2D" sheetId="3" r:id="rId3"/>
     <sheet name="Special Gaussian 2D" sheetId="4" r:id="rId4"/>
     <sheet name="LUTs - 2D" sheetId="5" r:id="rId5"/>
+    <sheet name="APX 0" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="55">
   <si>
     <t>Black</t>
   </si>
@@ -77,9 +78,6 @@
   </si>
   <si>
     <t>Fract bits</t>
-  </si>
-  <si>
-    <t>Comparison Between Fixed-Point Gaussian and Floating-Point Gaussian with Virtual Board 0 Approach</t>
   </si>
   <si>
     <t>Silicon Costs</t>
@@ -127,10 +125,82 @@
     <t>Gaussian Simulation - Fixed Point - 12 bits (8.4)</t>
   </si>
   <si>
-    <t>Gaussian Simulation - Fixed Point - 8 Fract bits — (10.8, 11.8, 11.8)</t>
+    <t>Gaussian Simulation - LUT- 8 Fract bits — (8.8)</t>
   </si>
   <si>
-    <t>Gaussian Simulation - LUT- 8 Fract bits — (8.8)</t>
+    <t>Aproximated Adders and Aproximated Multipliers (build with normal adders)</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - APX 0- 8 Fract bits — (8.8)</t>
+  </si>
+  <si>
+    <t>Comparison Between Fixed-Point Gaussian and Floating-Point Gaussian with Virtual Board 2 Approach</t>
+  </si>
+  <si>
+    <t>Comparison Between Approximated Gaussian and Floating-Point Gaussian with Virtual Board 2 Approach</t>
+  </si>
+  <si>
+    <t>Critical path: multiplier</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Arch</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>APX 0</t>
+  </si>
+  <si>
+    <t>APX 1</t>
+  </si>
+  <si>
+    <t>Normal mult and Apx_adder</t>
+  </si>
+  <si>
+    <t>APX 2</t>
+  </si>
+  <si>
+    <t>LUT mult and Apx_adder</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - APX 1- 8 Fract bits — (8.8)</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - APX 2- 8 Fract bits — (8.8)</t>
+  </si>
+  <si>
+    <t>Special Gaussian Simulation - Fixed Point - 8 Fract bits — (10.8, 11.8, 11.8)</t>
+  </si>
+  <si>
+    <t>APX 3</t>
+  </si>
+  <si>
+    <t>Gaussian Filter Arch</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Apx_multiplier and Apx_adder</t>
+  </si>
+  <si>
+    <t>Low PSNR</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - APX 3- 8 Fract bits — (8.8)</t>
+  </si>
+  <si>
+    <t>Window size</t>
   </si>
 </sst>
 </file>
@@ -142,7 +212,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +272,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -518,6 +602,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,8 +623,26 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7039,10 +7144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BA4AD1-F16F-4A97-9130-DD46CA139F38}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7070,7 +7175,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -7393,8 +7498,238 @@
         <v>44.264096579018997</v>
       </c>
     </row>
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="49"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="44"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="51"/>
+      <c r="F12" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="51"/>
+      <c r="J12" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="51"/>
+      <c r="L12" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="51"/>
+      <c r="N12" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="46"/>
+      <c r="P12" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="46"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>4</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="21"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>6</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="26">
+    <mergeCell ref="A10:S10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="N11:S11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="R12:S12"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -7418,7 +7753,7 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:I7"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7459,257 +7794,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
+      <c r="N1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="N1" s="55" t="s">
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="58"/>
+      <c r="AA1" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="57"/>
-      <c r="AA1" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="58"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
-      <c r="N2" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="60"/>
-      <c r="AA2" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="59"/>
-      <c r="AE2" s="59"/>
-      <c r="AF2" s="59"/>
-      <c r="AG2" s="59"/>
-      <c r="AH2" s="59"/>
-      <c r="AI2" s="59"/>
-      <c r="AJ2" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK2" s="59"/>
-      <c r="AL2" s="60"/>
+      <c r="A2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
+      <c r="N2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="61"/>
+      <c r="AA2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="60"/>
+      <c r="AF2" s="60"/>
+      <c r="AG2" s="60"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK2" s="60"/>
+      <c r="AL2" s="61"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="B3" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
       <c r="N3" s="26"/>
-      <c r="O3" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
+      <c r="O3" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
       <c r="W3" s="27"/>
       <c r="X3" s="27"/>
       <c r="Y3" s="28"/>
       <c r="AA3" s="26"/>
-      <c r="AB3" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="61"/>
-      <c r="AI3" s="61"/>
+      <c r="AB3" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="55"/>
+      <c r="AE3" s="55"/>
+      <c r="AF3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG3" s="55"/>
+      <c r="AH3" s="55"/>
+      <c r="AI3" s="55"/>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="27"/>
       <c r="AL3" s="28"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="L4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>25</v>
-      </c>
       <c r="N4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="P4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="Q4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="S4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="U4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="W4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="31" t="s">
+      <c r="Y4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="32" t="s">
-        <v>25</v>
-      </c>
       <c r="AA4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="31" t="s">
+      <c r="AC4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AC4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="AD4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AE4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="AF4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AG4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="AH4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AI4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="AJ4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AK4" s="31" t="s">
+      <c r="AL4" s="32" t="s">
         <v>24</v>
-      </c>
-      <c r="AL4" s="32" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -8098,6 +8433,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AA2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AF3:AI3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="N1:Y1"/>
@@ -8108,11 +8448,6 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="AA1:AL1"/>
-    <mergeCell ref="AA2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AB3:AE3"/>
-    <mergeCell ref="AF3:AI3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:I7">
     <cfRule type="dataBar" priority="3">
@@ -8210,8 +8545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC10A16-97E5-4B3B-8180-57C6E2637B68}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8229,93 +8564,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
+      <c r="A1" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
+      <c r="A2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="B3" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="L4" s="32" t="s">
         <v>24</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8500,8 +8835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22EFCDA-42FC-453B-A44E-ABE1C98A5C37}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8519,93 +8854,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
+      <c r="A1" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
+      <c r="A2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="B3" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>21</v>
-      </c>
       <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="L4" s="32" t="s">
         <v>24</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8783,4 +9118,1104 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D495193F-46E4-4DFD-BF85-BE1FEB18D686}">
+  <dimension ref="A1:T32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="58"/>
+      <c r="N2" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="60"/>
+      <c r="L3" s="61"/>
+      <c r="N3" s="62">
+        <v>3</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="62">
+        <v>17.986499999999999</v>
+      </c>
+      <c r="T3" s="67">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="28"/>
+      <c r="N4" s="62">
+        <v>3</v>
+      </c>
+      <c r="O4" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="67">
+        <v>16.803000000000001</v>
+      </c>
+      <c r="T4" s="67">
+        <v>0.27848000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="62">
+        <v>3</v>
+      </c>
+      <c r="O5" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="67">
+        <v>7.2189177353369898</v>
+      </c>
+      <c r="T5" s="67">
+        <v>0.839547467218833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="41">
+        <v>3</v>
+      </c>
+      <c r="B6" s="33">
+        <v>286</v>
+      </c>
+      <c r="C6" s="33">
+        <v>570</v>
+      </c>
+      <c r="D6" s="33">
+        <v>16352</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="34">
+        <f>B6/32070</f>
+        <v>8.9179918927346433E-3</v>
+      </c>
+      <c r="G6" s="34">
+        <f>C6/128300</f>
+        <v>4.4427123928293061E-3</v>
+      </c>
+      <c r="H6" s="34">
+        <f>D6/4065280</f>
+        <v>4.02235516372796E-3</v>
+      </c>
+      <c r="I6" s="34">
+        <f>E6/87</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="35">
+        <v>152.41999999999999</v>
+      </c>
+      <c r="K6" s="33">
+        <f>(512+A6-1)*(512+A6-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="L6" s="36">
+        <f>((1/(J6*10000000))*K6)*10000</f>
+        <v>1.7333683243668812</v>
+      </c>
+      <c r="N6" s="62">
+        <v>3</v>
+      </c>
+      <c r="O6" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="67">
+        <v>16.803000000000001</v>
+      </c>
+      <c r="T6" s="67">
+        <v>0.27848000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="41">
+        <v>5</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34">
+        <f t="shared" ref="F7:F8" si="0">B7/32070</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="34">
+        <f t="shared" ref="G7:G8" si="1">C7/128300</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="34">
+        <f t="shared" ref="H7:H8" si="2">D7/4065280</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="34">
+        <f t="shared" ref="I7:I8" si="3">E7/87</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="35"/>
+      <c r="K7" s="33">
+        <f>(512+A7-1)*(512+A7-1)+6</f>
+        <v>266262</v>
+      </c>
+      <c r="L7" s="36" t="e">
+        <f t="shared" ref="L7:L8" si="4">((1/(J7*10000000))*K7)*10000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="42">
+        <v>7</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="39"/>
+      <c r="K8" s="37">
+        <f>(512+A8-1)*(512+A8-1)+6</f>
+        <v>268330</v>
+      </c>
+      <c r="L8" s="40" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="58"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="60"/>
+      <c r="L11" s="61"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="28"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="41">
+        <v>3</v>
+      </c>
+      <c r="B14" s="33">
+        <v>199</v>
+      </c>
+      <c r="C14" s="33">
+        <v>444</v>
+      </c>
+      <c r="D14" s="33">
+        <v>16352</v>
+      </c>
+      <c r="E14" s="33">
+        <v>8</v>
+      </c>
+      <c r="F14" s="34">
+        <f>B14/32070</f>
+        <v>6.2051761771125665E-3</v>
+      </c>
+      <c r="G14" s="34">
+        <f>C14/128300</f>
+        <v>3.4606391270459859E-3</v>
+      </c>
+      <c r="H14" s="34">
+        <f>D14/4065280</f>
+        <v>4.02235516372796E-3</v>
+      </c>
+      <c r="I14" s="34">
+        <f>E14/87</f>
+        <v>9.1954022988505746E-2</v>
+      </c>
+      <c r="J14" s="35">
+        <v>261.57</v>
+      </c>
+      <c r="K14" s="33">
+        <f>(512+A14-1)*(512+A14-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="L14" s="36">
+        <f>((1/(J14*10000000))*K14)*10000</f>
+        <v>1.0100546698780442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="41">
+        <v>5</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34">
+        <f t="shared" ref="F15:F16" si="5">B15/32070</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="34">
+        <f t="shared" ref="G15:G16" si="6">C15/128300</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="34">
+        <f t="shared" ref="H15:H16" si="7">D15/4065280</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="34">
+        <f t="shared" ref="I15:I16" si="8">E15/87</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="35"/>
+      <c r="K15" s="33">
+        <f>(512+A15-1)*(512+A15-1)+6</f>
+        <v>266262</v>
+      </c>
+      <c r="L15" s="36" t="e">
+        <f t="shared" ref="L15:L16" si="9">((1/(J15*10000000))*K15)*10000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
+        <v>7</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="39"/>
+      <c r="K16" s="37">
+        <f>(512+A16-1)*(512+A16-1)+6</f>
+        <v>268330</v>
+      </c>
+      <c r="L16" s="40" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="58"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="60"/>
+      <c r="L19" s="61"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="41">
+        <v>3</v>
+      </c>
+      <c r="B22" s="33">
+        <v>215</v>
+      </c>
+      <c r="C22" s="33">
+        <v>471</v>
+      </c>
+      <c r="D22" s="33">
+        <v>16352</v>
+      </c>
+      <c r="E22" s="33">
+        <v>3</v>
+      </c>
+      <c r="F22" s="34">
+        <f>B22/32070</f>
+        <v>6.7040848144683503E-3</v>
+      </c>
+      <c r="G22" s="34">
+        <f>C22/128300</f>
+        <v>3.6710833982852688E-3</v>
+      </c>
+      <c r="H22" s="34">
+        <f>D22/4065280</f>
+        <v>4.02235516372796E-3</v>
+      </c>
+      <c r="I22" s="34">
+        <f>E22/87</f>
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="J22" s="35">
+        <v>266.67</v>
+      </c>
+      <c r="K22" s="33">
+        <f>(512+A22-1)*(512+A22-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="L22" s="36">
+        <f>((1/(J22*10000000))*K22)*10000</f>
+        <v>0.99073761577980279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="41">
+        <v>5</v>
+      </c>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34">
+        <f t="shared" ref="F23:F24" si="10">B23/32070</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="34">
+        <f t="shared" ref="G23:G24" si="11">C23/128300</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="34">
+        <f t="shared" ref="H23:H24" si="12">D23/4065280</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="34">
+        <f t="shared" ref="I23:I24" si="13">E23/87</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="35"/>
+      <c r="K23" s="33">
+        <f>(512+A23-1)*(512+A23-1)+6</f>
+        <v>266262</v>
+      </c>
+      <c r="L23" s="36" t="e">
+        <f t="shared" ref="L23:L24" si="14">((1/(J23*10000000))*K23)*10000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="42">
+        <v>7</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="38">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="38">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="39"/>
+      <c r="K24" s="37">
+        <f>(512+A24-1)*(512+A24-1)+6</f>
+        <v>268330</v>
+      </c>
+      <c r="L24" s="40" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="58"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="60"/>
+      <c r="L27" s="61"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="41">
+        <v>3</v>
+      </c>
+      <c r="B30" s="33">
+        <v>266</v>
+      </c>
+      <c r="C30" s="33">
+        <v>479</v>
+      </c>
+      <c r="D30" s="33">
+        <v>8176</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="34">
+        <f>B30/32070</f>
+        <v>8.2943560960399131E-3</v>
+      </c>
+      <c r="G30" s="34">
+        <f>C30/128300</f>
+        <v>3.7334372564302417E-3</v>
+      </c>
+      <c r="H30" s="34">
+        <f>D30/4065280</f>
+        <v>2.01117758186398E-3</v>
+      </c>
+      <c r="I30" s="34">
+        <f>E30/87</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="35">
+        <v>279.10000000000002</v>
+      </c>
+      <c r="K30" s="33">
+        <f>(512+A30-1)*(512+A30-1)+4</f>
+        <v>264200</v>
+      </c>
+      <c r="L30" s="36">
+        <f>((1/(J30*10000000))*K30)*10000</f>
+        <v>0.94661411680401286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="41">
+        <v>5</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34">
+        <f t="shared" ref="F31:F32" si="15">B31/32070</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="34">
+        <f t="shared" ref="G31:G32" si="16">C31/128300</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" ref="H31:H32" si="17">D31/4065280</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="34">
+        <f t="shared" ref="I31:I32" si="18">E31/87</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="35"/>
+      <c r="K31" s="33">
+        <f>(512+A31-1)*(512+A31-1)+6</f>
+        <v>266262</v>
+      </c>
+      <c r="L31" s="36" t="e">
+        <f t="shared" ref="L31:L32" si="19">((1/(J31*10000000))*K31)*10000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="42">
+        <v>7</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="38">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="38">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="39"/>
+      <c r="K32" s="37">
+        <f>(512+A32-1)*(512+A32-1)+6</f>
+        <v>268330</v>
+      </c>
+      <c r="L32" s="40" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F6:I8">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{49A8F500-C8F3-4423-9094-1EE1070AD53F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:I16">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0BFB7261-4162-41A9-B7EE-9F6B9B3756CB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:I24">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F6E836C5-0BA2-4EFE-86C1-8968FD81A99C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:I32">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{06EA3E92-EDCA-45CA-825E-562C02CB708B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{49A8F500-C8F3-4423-9094-1EE1070AD53F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F6:I8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0BFB7261-4162-41A9-B7EE-9F6B9B3756CB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F14:I16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F6E836C5-0BA2-4EFE-86C1-8968FD81A99C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F22:I24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{06EA3E92-EDCA-45CA-825E-562C02CB708B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F30:I32</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Problems in Separable Filter 5x5
</commit_message>
<xml_diff>
--- a/Results/Results_python.xlsx
+++ b/Results/Results_python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5927951\Documents\Univali\TTC\TTCIII\Project\Architecture-of-FPGA-based-Systems-for-Digital-Image-Processing\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BB821C-DD8B-446A-A178-CF8AF69D0B33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A77355F-C838-4093-A0AC-B2EE3B0113C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-4470" windowWidth="25440" windowHeight="15540" activeTab="5" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
+    <workbookView xWindow="-25320" yWindow="-4470" windowWidth="25440" windowHeight="15540" firstSheet="1" activeTab="6" xr2:uid="{6520BC44-3547-42BA-B099-3EF3D97F4FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Virtual Board" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Special Gaussian 2D" sheetId="4" r:id="rId4"/>
     <sheet name="LUTs - 2D" sheetId="5" r:id="rId5"/>
     <sheet name="APX 0" sheetId="6" r:id="rId6"/>
+    <sheet name="Planilha1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="56">
   <si>
     <t>Black</t>
   </si>
@@ -201,6 +202,9 @@
   </si>
   <si>
     <t>Window size</t>
+  </si>
+  <si>
+    <t>Gaussian Simulation - SEP- 8 Fract bits — (9.8)</t>
   </si>
 </sst>
 </file>
@@ -448,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,6 +570,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,9 +624,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,26 +642,20 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6797,93 +6810,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="57"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="43" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="44"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="52"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="50" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="50" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="50" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="50" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
+      <c r="Q3" s="54"/>
+      <c r="R3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="46"/>
+      <c r="S3" s="54"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -7174,93 +7187,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="57"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="43" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="44"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="52"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="50" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="50" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="50" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="50" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
+      <c r="Q3" s="54"/>
+      <c r="R3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="46"/>
+      <c r="S3" s="54"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -7499,93 +7512,93 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="49"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="57"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="53" t="s">
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="43" t="s">
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="44"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="52"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="50" t="s">
+      <c r="C12" s="59"/>
+      <c r="D12" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="50" t="s">
+      <c r="E12" s="59"/>
+      <c r="F12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="50" t="s">
+      <c r="G12" s="59"/>
+      <c r="H12" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="51"/>
-      <c r="J12" s="50" t="s">
+      <c r="I12" s="59"/>
+      <c r="J12" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="50" t="s">
+      <c r="K12" s="59"/>
+      <c r="L12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="51"/>
-      <c r="N12" s="45" t="s">
+      <c r="M12" s="59"/>
+      <c r="N12" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="46"/>
-      <c r="P12" s="45" t="s">
+      <c r="O12" s="54"/>
+      <c r="P12" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="45" t="s">
+      <c r="Q12" s="54"/>
+      <c r="R12" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="46"/>
+      <c r="S12" s="54"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -7717,6 +7730,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="A10:S10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="H11:M11"/>
@@ -7730,19 +7756,6 @@
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="R12:S12"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -7794,145 +7807,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="58"/>
-      <c r="N1" s="56" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="65"/>
+      <c r="N1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="58"/>
-      <c r="AA1" s="56" t="s">
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="65"/>
+      <c r="AA1" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="58"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="64"/>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="65"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
-      <c r="N2" s="59" t="s">
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
+      <c r="N2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60" t="s">
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
-      <c r="AA2" s="59" t="s">
+      <c r="X2" s="67"/>
+      <c r="Y2" s="68"/>
+      <c r="AA2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60" t="s">
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="61"/>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="68"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
       <c r="N3" s="26"/>
-      <c r="O3" s="55" t="s">
+      <c r="O3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55" t="s">
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
       <c r="W3" s="27"/>
       <c r="X3" s="27"/>
       <c r="Y3" s="28"/>
       <c r="AA3" s="26"/>
-      <c r="AB3" s="55" t="s">
+      <c r="AB3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55" t="s">
+      <c r="AC3" s="69"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="69"/>
+      <c r="AF3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="55"/>
+      <c r="AG3" s="69"/>
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="69"/>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="27"/>
       <c r="AL3" s="28"/>
@@ -8433,11 +8446,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AA1:AL1"/>
-    <mergeCell ref="AA2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AB3:AE3"/>
-    <mergeCell ref="AF3:AI3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="N1:Y1"/>
@@ -8448,6 +8456,11 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="A1:L1"/>
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AA2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AF3:AI3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:I7">
     <cfRule type="dataBar" priority="3">
@@ -8564,53 +8577,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="58"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
@@ -8854,53 +8867,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="58"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="28"/>
@@ -9124,8 +9137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D495193F-46E4-4DFD-BF85-BE1FEB18D686}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9150,130 +9163,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="58"/>
-      <c r="N2" s="70" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="N2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="68" t="s">
+      <c r="O2" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="68" t="s">
+      <c r="P2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="68" t="s">
+      <c r="Q2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="69" t="s">
+      <c r="R2" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="68" t="s">
+      <c r="S2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="68" t="s">
+      <c r="T2" s="48" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="61"/>
-      <c r="N3" s="62">
+      <c r="K3" s="67"/>
+      <c r="L3" s="68"/>
+      <c r="N3" s="43">
         <v>3</v>
       </c>
-      <c r="O3" s="64" t="s">
+      <c r="O3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="Q3" s="62" t="s">
+      <c r="Q3" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="62" t="s">
+      <c r="R3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="62">
+      <c r="S3" s="43">
         <v>17.986499999999999</v>
       </c>
-      <c r="T3" s="67">
+      <c r="T3" s="47">
         <v>0.24299999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
       <c r="L4" s="28"/>
-      <c r="N4" s="62">
+      <c r="N4" s="43">
         <v>3</v>
       </c>
-      <c r="O4" s="64" t="s">
+      <c r="O4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="P4" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="62" t="s">
+      <c r="R4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="67">
+      <c r="S4" s="47">
         <v>16.803000000000001</v>
       </c>
-      <c r="T4" s="67">
+      <c r="T4" s="47">
         <v>0.27848000000000001</v>
       </c>
     </row>
@@ -9314,25 +9327,25 @@
       <c r="L5" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="62">
+      <c r="N5" s="43">
         <v>3</v>
       </c>
-      <c r="O5" s="64" t="s">
+      <c r="O5" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="66" t="s">
+      <c r="Q5" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="R5" s="62" t="s">
+      <c r="R5" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="S5" s="67">
+      <c r="S5" s="47">
         <v>7.2189177353369898</v>
       </c>
-      <c r="T5" s="67">
+      <c r="T5" s="47">
         <v>0.839547467218833</v>
       </c>
     </row>
@@ -9379,25 +9392,25 @@
         <f>((1/(J6*10000000))*K6)*10000</f>
         <v>1.7333683243668812</v>
       </c>
-      <c r="N6" s="62">
+      <c r="N6" s="43">
         <v>3</v>
       </c>
-      <c r="O6" s="64" t="s">
+      <c r="O6" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="P6" s="64" t="s">
+      <c r="P6" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="66" t="s">
+      <c r="Q6" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="62" t="s">
+      <c r="R6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="S6" s="67">
+      <c r="S6" s="47">
         <v>16.803000000000001</v>
       </c>
-      <c r="T6" s="67">
+      <c r="T6" s="47">
         <v>0.27848000000000001</v>
       </c>
     </row>
@@ -9470,53 +9483,53 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60" t="s">
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="60"/>
-      <c r="L11" s="61"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="68"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
       <c r="L12" s="28"/>
@@ -9558,8 +9571,8 @@
       <c r="L13" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
@@ -9674,53 +9687,53 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="58"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="65"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60" t="s">
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="61"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="68"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
       <c r="L20" s="28"/>
@@ -9876,53 +9889,53 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="58"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="65"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60" t="s">
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="60"/>
-      <c r="L27" s="61"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="68"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55" t="s">
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
       <c r="L28" s="28"/>
@@ -10079,6 +10092,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="A19:I19"/>
@@ -10088,18 +10113,6 @@
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="J27:L27"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I8">
     <cfRule type="dataBar" priority="4">
@@ -10218,4 +10231,287 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F800A3E-2A25-4F32-95CF-F58BDC1950FC}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="65"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="41">
+        <v>3</v>
+      </c>
+      <c r="B5" s="33">
+        <v>234</v>
+      </c>
+      <c r="C5" s="33">
+        <v>505</v>
+      </c>
+      <c r="D5" s="33">
+        <v>17.306000000000001</v>
+      </c>
+      <c r="E5" s="33">
+        <v>5</v>
+      </c>
+      <c r="F5" s="34">
+        <f>B5/32070</f>
+        <v>7.2965388213283439E-3</v>
+      </c>
+      <c r="G5" s="34">
+        <f>C5/128300</f>
+        <v>3.9360872954014026E-3</v>
+      </c>
+      <c r="H5" s="34">
+        <f>D5/4065280</f>
+        <v>4.2570253463476074E-6</v>
+      </c>
+      <c r="I5" s="34">
+        <f>E5/87</f>
+        <v>5.7471264367816091E-2</v>
+      </c>
+      <c r="J5" s="35">
+        <v>239.52</v>
+      </c>
+      <c r="K5" s="33">
+        <f>(512+A5-1)*(512+A5-1)+7</f>
+        <v>264203</v>
+      </c>
+      <c r="L5" s="36">
+        <f>((1/(J5*10000000))*K5)*10000</f>
+        <v>1.1030519372077487</v>
+      </c>
+      <c r="M5" s="73">
+        <v>58.117841746937202</v>
+      </c>
+      <c r="N5" s="73">
+        <v>2.3938616932929202E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="41">
+        <v>5</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34">
+        <f t="shared" ref="F6:F7" si="0">B6/32070</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="34">
+        <f t="shared" ref="G6:G7" si="1">C6/128300</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="34">
+        <f t="shared" ref="H6:H7" si="2">D6/4065280</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="34">
+        <f t="shared" ref="I6:I7" si="3">E6/87</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="33">
+        <f>(512+A6-1)*(512+A6-1)+6</f>
+        <v>266262</v>
+      </c>
+      <c r="L6" s="36" t="e">
+        <f t="shared" ref="L6:L7" si="4">((1/(J6*10000000))*K6)*10000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="42">
+        <v>7</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="39"/>
+      <c r="K7" s="37">
+        <f>(512+A7-1)*(512+A7-1)+6</f>
+        <v>268330</v>
+      </c>
+      <c r="L7" s="40" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F5:I7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{43EEF4D6-8BDF-4DDE-A93A-4C5B2684B721}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{43EEF4D6-8BDF-4DDE-A93A-4C5B2684B721}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F5:I7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>